<commit_message>
files for Precious, box rooted
</commit_message>
<xml_diff>
--- a/machines/precious/preciousMeth.xlsx
+++ b/machines/precious/preciousMeth.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Recon" sheetId="1" state="visible" r:id="rId3"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t xml:space="preserve">Don’t Forget</t>
   </si>
@@ -50,6 +50,12 @@
     <t xml:space="preserve">sudo -l</t>
   </si>
   <si>
+    <t xml:space="preserve">henry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3c1AqGHtoI0aXAYFH</t>
+  </si>
+  <si>
     <t xml:space="preserve">gtfo bins</t>
   </si>
   <si>
@@ -59,142 +65,76 @@
     <t xml:space="preserve">Burp</t>
   </si>
   <si>
+    <t xml:space="preserve">netstat (ss)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/UNICORDev/exploit-CVE-2022-25765?tab=readme-ov-file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">╔══════════╣ Active Ports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">╚ https://book.hacktricks.xyz/linux-hardening/privilege-escalation#open-ports                                                                                                                                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcp        0      0 0.0.0.0:80              0.0.0.0:*               LISTEN      -                                                                                                                                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcp        0      0 0.0.0.0:22              0.0.0.0:*               LISTEN      -                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcp        0      0 127.0.0.1:46857         0.0.0.0:*               LISTEN      843/Passenger RubyA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcp6       0      0 :::80                   :::*                    LISTEN      -                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcp6       0      0 :::22                   :::*                    LISTEN      -                   </t>
+  </si>
+  <si>
     <t xml:space="preserve">sudo nmap $TIP -A -p-  -oA $TIP-A-p- </t>
   </si>
   <si>
-    <t xml:space="preserve">Not shown: 65531 closed tcp ports (reset)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PORT      STATE    SERVICE VERSION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2222/tcp  open     ssh     (protocol 2.0)</t>
+    <t xml:space="preserve">Starting Nmap 7.94SVN ( https://nmap.org ) at 2024-09-28 21:16 EDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nmap scan report for 10.10.11.189</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Host is up (0.056s latency).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not shown: 65533 closed tcp ports (reset)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PORT   STATE SERVICE VERSION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22/tcp open  ssh     OpenSSH 8.4p1 Debian 5+deb11u1 (protocol 2.0)</t>
   </si>
   <si>
     <t xml:space="preserve">| ssh-hostkey: </t>
   </si>
   <si>
-    <t xml:space="preserve">|_  2048 71:90:e3:a7:c9:5d:83:66:34:88:3d:eb:b4:c7:88:fb (RSA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">| fingerprint-strings: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">|   NULL: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">|_    SSH-2.0-SSH Server - Banana Studio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5555/tcp  filtered freeciv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35917/tcp open     unknown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|   GenericLines: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     HTTP/1.0 400 Bad Request</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     Date: Fri, 27 Sep 2024 20:13:40 GMT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     Content-Length: 22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     Content-Type: text/plain; charset=US-ASCII</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     Connection: Close</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     Invalid request line:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|   GetRequest: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     HTTP/1.1 412 Precondition Failed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     Content-Length: 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|   HTTPOptions: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     HTTP/1.0 501 Not Implemented</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     Date: Fri, 27 Sep 2024 20:13:45 GMT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     Content-Length: 29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     Method not supported: OPTIONS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|   Help: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     Date: Fri, 27 Sep 2024 20:14:01 GMT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     Content-Length: 26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     Invalid request line: HELP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|   RTSPRequest: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     Content-Length: 39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     valid protocol version: RTSP/1.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|   SSLSessionReq: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     Content-Length: 73</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     Invalid request line: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     ?G???,???`~?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     ??{????w????&lt;=?o?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|   TLSSessionReq: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     Content-Length: 71</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     ??random1random2random3random4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|   TerminalServerCookie: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">|     Content-Length: 54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|_    Cookie: mstshash=nmap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">59777/tcp open     http    Bukkit JSONAPI httpd for Minecraft game server 3.6.0 or older</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|_http-title: Site doesn't have a title (text/plain).</t>
+    <t xml:space="preserve">|   3072 84:5e:13:a8:e3:1e:20:66:1d:23:55:50:f6:30:47:d2 (RSA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|   256 a2:ef:7b:96:65:ce:41:61:c4:67:ee:4e:96:c7:c8:92 (ECDSA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|_  256 33:05:3d:cd:7a:b7:98:45:82:39:e7:ae:3c:91:a6:58 (ED25519)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80/tcp open  http    nginx 1.18.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|_http-title: Did not follow redirect to http://precious.htb/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|_http-server-header: nginx/1.18.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No exact OS matches for host (If you know what OS is running on it, see https://nmap.org/submit/ ).</t>
   </si>
   <si>
     <t xml:space="preserve">sudo nmap -p 25 --script smtp-enum-users $TIP</t>
@@ -206,6 +146,42 @@
     <t xml:space="preserve">curl -I $TURL -k</t>
   </si>
   <si>
+    <t xml:space="preserve">HTTP/1.1 200 OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content-Type: text/html;charset=utf-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content-Length: 483</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connection: keep-alive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status: 200 OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X-XSS-Protection: 1; mode=block</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X-Content-Type-Options: nosniff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X-Frame-Options: SAMEORIGIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date: Sun, 29 Sep 2024 03:25:19 GMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X-Powered-By: Phusion Passenger(R) 6.0.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Server: nginx/1.18.0 + Phusion Passenger(R) 6.0.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X-Runtime: Ruby</t>
+  </si>
+  <si>
     <t xml:space="preserve">sudo gobuster dir -u $TURL -w /usr/share/dirbuster/wordlists/directory-list-2.3-medium.txt</t>
   </si>
   <si>
@@ -225,6 +201,18 @@
   </si>
   <si>
     <t xml:space="preserve">sudo nikto -h $TURL -o niktoResult.txt -Format txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nginx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.18.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PhusionPassenger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.0.15</t>
   </si>
 </sst>
 </file>
@@ -234,7 +222,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +252,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -331,11 +325,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -343,7 +333,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -536,15 +530,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -565,23 +560,72 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="H2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -600,25 +644,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G10" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -728,376 +786,166 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:A1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="260.95"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="2" style="4" width="8.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="10.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="4" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="260.95"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="2" style="1" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.86"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="1" width="8.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>8</v>
+      <c r="A1" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>9</v>
+      <c r="A3" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>11</v>
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="7"/>
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>14</v>
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>15</v>
+      <c r="A9" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>14</v>
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
-        <v>19</v>
+      <c r="A14" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>20</v>
+      <c r="A15" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
+      <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="71" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
+    <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1114,10 +962,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1127,7 +975,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>54</v>
+        <v>34</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1143,9 +994,7 @@
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="A14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1170,10 +1019,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1183,7 +1032,67 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>56</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1212,7 +1121,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1343,18 +1252,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1386,7 +1295,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1415,7 +1324,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>